<commit_message>
Updated Lookup table and start of report
</commit_message>
<xml_diff>
--- a/4-5-2017/Experimental Setup_Constant_Current_4-5-2017.xlsx
+++ b/4-5-2017/Experimental Setup_Constant_Current_4-5-2017.xlsx
@@ -1326,11 +1326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="366796192"/>
-        <c:axId val="364780656"/>
+        <c:axId val="44911840"/>
+        <c:axId val="128041728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="366796192"/>
+        <c:axId val="44911840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,12 +1443,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364780656"/>
+        <c:crossAx val="128041728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="364780656"/>
+        <c:axId val="128041728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1561,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366796192"/>
+        <c:crossAx val="44911840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1677,7 +1677,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Load Torque and Motor Speed behaviour at constant current</a:t>
+              <a:t>Load Torque vs Motor Speed at constant values of Supply Current</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3584,11 +3584,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363523824"/>
-        <c:axId val="363522704"/>
+        <c:axId val="128048448"/>
+        <c:axId val="128049008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="363523824"/>
+        <c:axId val="128048448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3701,12 +3701,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363522704"/>
+        <c:crossAx val="128049008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="363522704"/>
+        <c:axId val="128049008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3747,7 +3747,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Load Torque (ft-lb)</a:t>
+                  <a:t>Load Torque (lb-ft)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3819,7 +3819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363523824"/>
+        <c:crossAx val="128048448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5847,11 +5847,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="345068752"/>
-        <c:axId val="345069312"/>
+        <c:axId val="128055728"/>
+        <c:axId val="128056288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="345068752"/>
+        <c:axId val="128055728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5964,12 +5964,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345069312"/>
+        <c:crossAx val="128056288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="345069312"/>
+        <c:axId val="128056288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6082,7 +6082,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345068752"/>
+        <c:crossAx val="128055728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7819,7 +7819,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4C09AB4-C840-42C5-A72D-C1EEE0C3A78E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4C09AB4-C840-42C5-A72D-C1EEE0C3A78E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7857,7 +7857,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4C09AB4-C840-42C5-A72D-C1EEE0C3A78E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4C09AB4-C840-42C5-A72D-C1EEE0C3A78E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7895,7 +7895,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4C09AB4-C840-42C5-A72D-C1EEE0C3A78E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4C09AB4-C840-42C5-A72D-C1EEE0C3A78E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8185,7 +8185,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:L1048576"/>
+      <selection pane="bottomLeft" activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>